<commit_message>
28-02-2023 -> Scripting DPLKKPS123-001 until DPLKKPS125-001, DPLKKPS128-001, DPLKKPS131-001 until DPLKKPS132-002
01-03-2023
-> Scripting DPLKKPS120-001, DPLKKPS121-001, DPLKKPS133-001 until DPLKKPS134-002, DPLKKPS151-001, DPLKKPS154-001
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV127-001 - Investasi - Fixed Income - Cetak Dealing Ticket Order Fixed Income.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKINV127-001 - Investasi - Fixed Income - Cetak Dealing Ticket Order Fixed Income.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92B19FB-FE75-42FF-A53D-A032666802CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC81B119-0D9E-4E29-8BCA-99893AEA6D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -525,7 +525,7 @@
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="O2" sqref="O2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>